<commit_message>
Correct gain, write energy test
</commit_message>
<xml_diff>
--- a/tests/mobile_network/link_budget_validation.xlsx
+++ b/tests/mobile_network/link_budget_validation.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\digital_comms\tests\mobile_network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185710D1-F8FE-43E1-9059-59A62687DE56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E2D58A-958C-4983-8375-16E8D024D299}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="link_buget_example 1" sheetId="1" r:id="rId1"/>
+    <sheet name="4G-5G CM LUT" sheetId="2" r:id="rId2"/>
+    <sheet name="Energy_consumption" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
   <si>
     <t>Rx Power (dBm)</t>
   </si>
@@ -86,9 +88,6 @@
     <t>Calculate I + N</t>
   </si>
   <si>
-    <t>CalculateSINR</t>
-  </si>
-  <si>
     <t>Spectral efficiency</t>
   </si>
   <si>
@@ -129,17 +128,110 @@
   </si>
   <si>
     <t>Calculate receiver received power</t>
+  </si>
+  <si>
+    <t>SINR (dB)</t>
+  </si>
+  <si>
+    <t>Calculate SINR</t>
+  </si>
+  <si>
+    <t>CQI index</t>
+  </si>
+  <si>
+    <t>4G LTE (Zarrinkoub, 2014)</t>
+  </si>
+  <si>
+    <t>5G (ETSI, 2018)</t>
+  </si>
+  <si>
+    <t>Modulation</t>
+  </si>
+  <si>
+    <t>Code rate x 1024</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>QPSK</t>
+  </si>
+  <si>
+    <t>16QAM</t>
+  </si>
+  <si>
+    <t>64QAM</t>
+  </si>
+  <si>
+    <t>256QAM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zarrinkoub, Houman. 2014. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Understanding LTE with MATLAB: From Mathematical Modeling to Simulation and Prototyping</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>. John Wiley &amp; Sons.</t>
+    </r>
+  </si>
+  <si>
+    <t>ETSI. 2018. ‘5G; NR; Physical Layer Procedures for Data (3GPP TS 38.214 Version 15.3.0 Release 15)’. Valbonne, France: ETSI.</t>
+  </si>
+  <si>
+    <t>Energy consumption</t>
+  </si>
+  <si>
+    <t>Power (dBm)</t>
+  </si>
+  <si>
+    <t>Power linear (watts)</t>
+  </si>
+  <si>
+    <t>Power per site (watts)</t>
+  </si>
+  <si>
+    <t>Total power per area (watts)</t>
+  </si>
+  <si>
+    <t>Throughput per area (bps per km^2)</t>
+  </si>
+  <si>
+    <t>Energy efficiency (bps/watt)</t>
+  </si>
+  <si>
+    <t>Cells per site (watts)</t>
+  </si>
+  <si>
+    <t>Sites per area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -184,6 +276,34 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,7 +313,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -291,12 +411,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -343,26 +570,99 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -679,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +995,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -708,7 +1008,7 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -727,16 +1027,16 @@
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>(B3+C3-D3)-E3-F3+G3-H3</f>
-        <v>-45.44</v>
+        <v>-48.44</v>
       </c>
       <c r="B3" s="6">
         <v>40</v>
       </c>
       <c r="C3" s="6">
-        <v>20</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
       </c>
       <c r="E3" s="6">
         <v>99.44</v>
@@ -762,55 +1062,55 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="28">
         <f>(B9+C9-D9)-E9-F9+G9-H9</f>
-        <v>-65.959999999999994</v>
-      </c>
-      <c r="B9" s="6">
+        <v>-68.959999999999994</v>
+      </c>
+      <c r="B9" s="29">
         <v>40</v>
       </c>
-      <c r="C9" s="6">
-        <v>20</v>
-      </c>
-      <c r="D9" s="6">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="C9" s="29">
+        <v>16</v>
+      </c>
+      <c r="D9" s="29">
+        <v>1</v>
+      </c>
+      <c r="E9" s="29">
         <v>119.96</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="29">
         <v>4</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="29">
         <v>4</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="30">
         <v>4</v>
       </c>
     </row>
@@ -827,55 +1127,55 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="28">
         <f>(B12+C12-D12)-E12-F12+G12-H12</f>
-        <v>-66.02</v>
-      </c>
-      <c r="B12" s="6">
+        <v>-69.02</v>
+      </c>
+      <c r="B12" s="29">
         <v>40</v>
       </c>
-      <c r="C12" s="6">
-        <v>20</v>
-      </c>
-      <c r="D12" s="6">
-        <v>2</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="C12" s="29">
+        <v>16</v>
+      </c>
+      <c r="D12" s="29">
+        <v>1</v>
+      </c>
+      <c r="E12" s="29">
         <v>120.02</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="29">
         <v>4</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="29">
         <v>4</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="30">
         <v>4</v>
       </c>
     </row>
@@ -901,7 +1201,7 @@
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -920,16 +1220,16 @@
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>(B15+C15-D15)-E15-F15+G15-H15</f>
-        <v>-78.400000000000006</v>
+        <v>-81.400000000000006</v>
       </c>
       <c r="B15" s="6">
         <v>40</v>
       </c>
       <c r="C15" s="6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D15" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="6">
         <v>132.4</v>
@@ -968,16 +1268,16 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1013,28 +1313,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <f>B25+C25</f>
-        <v>3.0772061732475448E-66</v>
+        <v>3.0772061732475449E-69</v>
       </c>
       <c r="B25" s="13">
         <f>SUM(POWER(10, A9),POWER(10, A12),POWER(10, A15))*(1+(D25/100))</f>
-        <v>3.0772061732475448E-66</v>
+        <v>3.0772061732475449E-69</v>
       </c>
       <c r="C25" s="13">
         <f>POWER(10, A20)</f>
@@ -1046,18 +1346,18 @@
     </row>
     <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1067,21 +1367,21 @@
       </c>
       <c r="B30" s="13">
         <f>POWER(10,A3)</f>
-        <v>3.6307805477009904E-46</v>
+        <v>3.6307805477009909E-49</v>
       </c>
       <c r="C30" s="16">
         <f>A25</f>
-        <v>3.0772061732475448E-66</v>
+        <v>3.0772061732475449E-69</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>15</v>
@@ -1098,52 +1398,30 @@
     </row>
     <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>15</v>
+      <c r="C39" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12">
-        <v>6.2266000000000004</v>
-      </c>
-      <c r="B40" s="16">
+      <c r="A40" s="24">
+        <f>B40*C40</f>
+        <v>62266000</v>
+      </c>
+      <c r="B40" s="31">
         <f>A35</f>
         <v>6.2266000000000004</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="24">
-        <f>B45*C45</f>
-        <v>62266000</v>
-      </c>
-      <c r="B45" s="6">
-        <f>A40</f>
-        <v>6.2266000000000004</v>
-      </c>
-      <c r="C45" s="23">
+      <c r="C40" s="23">
         <f>E20</f>
         <v>10000000</v>
       </c>
@@ -1152,4 +1430,566 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638A3F84-9186-47E2-B75B-D0A8861F43CA}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="49"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
+        <v>1</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="33">
+        <v>7.6200000000000004E-2</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="33">
+        <v>78</v>
+      </c>
+      <c r="G3" s="33">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="H3" s="35">
+        <v>-6.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <v>2</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0.1172</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0.2344</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="33">
+        <v>193</v>
+      </c>
+      <c r="G4" s="33">
+        <v>0.377</v>
+      </c>
+      <c r="H4" s="35">
+        <v>-4.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="34">
+        <v>3</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0.1885</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0.377</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="33">
+        <v>449</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0.877</v>
+      </c>
+      <c r="H5" s="35">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>4</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="33">
+        <v>308</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0.60160000000000002</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="33">
+        <v>378</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1.4765999999999999</v>
+      </c>
+      <c r="H6" s="35">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
+        <v>5</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="33">
+        <v>449</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0.877</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="33">
+        <v>490</v>
+      </c>
+      <c r="G7" s="33">
+        <v>1.9140999999999999</v>
+      </c>
+      <c r="H7" s="35">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>6</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="33">
+        <v>602</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1.1758</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="33">
+        <v>616</v>
+      </c>
+      <c r="G8" s="33">
+        <v>2.4062999999999999</v>
+      </c>
+      <c r="H8" s="35">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
+        <v>7</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="33">
+        <v>378</v>
+      </c>
+      <c r="D9" s="33">
+        <v>1.4765999999999999</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="33">
+        <v>466</v>
+      </c>
+      <c r="G9" s="33">
+        <v>2.7305000000000001</v>
+      </c>
+      <c r="H9" s="35">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <v>8</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="33">
+        <v>490</v>
+      </c>
+      <c r="D10" s="33">
+        <v>1.9140999999999999</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="33">
+        <v>567</v>
+      </c>
+      <c r="G10" s="33">
+        <v>3.3222999999999998</v>
+      </c>
+      <c r="H10" s="35">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="34">
+        <v>9</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="33">
+        <v>616</v>
+      </c>
+      <c r="D11" s="33">
+        <v>2.4062999999999999</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="33">
+        <v>666</v>
+      </c>
+      <c r="G11" s="33">
+        <v>3.9022999999999999</v>
+      </c>
+      <c r="H11" s="35">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="34">
+        <v>10</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="33">
+        <v>466</v>
+      </c>
+      <c r="D12" s="33">
+        <v>2.7305000000000001</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="33">
+        <v>772</v>
+      </c>
+      <c r="G12" s="33">
+        <v>4.5233999999999996</v>
+      </c>
+      <c r="H12" s="35">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <v>11</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="33">
+        <v>567</v>
+      </c>
+      <c r="D13" s="33">
+        <v>3.3222999999999998</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="33">
+        <v>873</v>
+      </c>
+      <c r="G13" s="33">
+        <v>5.1151999999999997</v>
+      </c>
+      <c r="H13" s="35">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>12</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="33">
+        <v>666</v>
+      </c>
+      <c r="D14" s="33">
+        <v>3.9022999999999999</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="33">
+        <v>711</v>
+      </c>
+      <c r="G14" s="33">
+        <v>5.5547000000000004</v>
+      </c>
+      <c r="H14" s="35">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
+        <v>13</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="33">
+        <v>772</v>
+      </c>
+      <c r="D15" s="33">
+        <v>4.5233999999999996</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="33">
+        <v>797</v>
+      </c>
+      <c r="G15" s="33">
+        <v>6.2266000000000004</v>
+      </c>
+      <c r="H15" s="35">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="34">
+        <v>14</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="33">
+        <v>873</v>
+      </c>
+      <c r="D16" s="33">
+        <v>5.1151999999999997</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="33">
+        <v>885</v>
+      </c>
+      <c r="G16" s="33">
+        <v>6.9141000000000004</v>
+      </c>
+      <c r="H16" s="35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="36">
+        <v>15</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="37">
+        <v>948</v>
+      </c>
+      <c r="D17" s="37">
+        <v>5.5547000000000004</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="37">
+        <v>948</v>
+      </c>
+      <c r="G17" s="37">
+        <v>7.4062999999999999</v>
+      </c>
+      <c r="H17" s="38">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C36E160-2DE2-4BD6-B8A4-FCF373663928}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41">
+        <v>40</v>
+      </c>
+      <c r="B3" s="6">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="41">
+        <f>POWER(10, A3/10)/1000</f>
+        <v>10</v>
+      </c>
+      <c r="B6" s="6">
+        <f>A6*B3</f>
+        <v>30</v>
+      </c>
+      <c r="C6" s="7">
+        <f>B6*C3</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="41">
+        <v>60000000</v>
+      </c>
+      <c r="B9" s="42">
+        <f>C6/A9</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>